<commit_message>
Added label form component.
</commit_message>
<xml_diff>
--- a/src/main/resources/example-form.xlsx
+++ b/src/main/resources/example-form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,11 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
   <si>
+    <t xml:space="preserve">Label</t>
+  </si>
+  <si>
     <t xml:space="preserve">Text</t>
   </si>
   <si>
@@ -34,7 +37,7 @@
     <t xml:space="preserve">Confirm Email</t>
   </si>
   <si>
-    <t xml:space="preserve">Eq(2)</t>
+    <t xml:space="preserve">Eq(4)</t>
   </si>
   <si>
     <t xml:space="preserve">Password</t>
@@ -138,31 +141,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="n">
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -175,25 +178,58 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>4</v>
+      <c r="B3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pattern validation and a small refactor.
</commit_message>
<xml_diff>
--- a/src/main/resources/example-form.xlsx
+++ b/src/main/resources/example-form.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -28,10 +28,19 @@
     <t xml:space="preserve">Label</t>
   </si>
   <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
     <t xml:space="preserve">Text</t>
   </si>
   <si>
+    <t xml:space="preserve">[a-zA-Z0-9]*</t>
+  </si>
+  <si>
     <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[a-zA-Z0-9]*@[a-zA-Z0-9]*</t>
   </si>
   <si>
     <t xml:space="preserve">Confirm Email</t>
@@ -141,26 +150,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>1</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -168,68 +184,86 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>3</v>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>5</v>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>6</v>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>